<commit_message>
Aanwezigheid Update week 2
</commit_message>
<xml_diff>
--- a/Aanwezigheid_RaceGame.xlsx
+++ b/Aanwezigheid_RaceGame.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\derek\Desktop\Race Game\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B10C0EDE-441F-4649-B1ED-EB77B8F0A99B}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A4D9B3C-BD00-47DD-9D4F-4A213E0E6104}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -23,6 +23,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -64,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="30">
   <si>
     <t>Aanwezigheid</t>
   </si>
@@ -142,6 +143,18 @@
   </si>
   <si>
     <t>Stefan</t>
+  </si>
+  <si>
+    <t>19/11/2018</t>
+  </si>
+  <si>
+    <t>20/11/2018</t>
+  </si>
+  <si>
+    <t>22/11/2018</t>
+  </si>
+  <si>
+    <t>23/11/2018</t>
   </si>
 </sst>
 </file>
@@ -1369,7 +1382,7 @@
   <dimension ref="A1:CM157"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="O10" sqref="O10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1461,17 +1474,17 @@
         <v>21</v>
       </c>
       <c r="I2" s="54"/>
-      <c r="J2" s="54">
-        <v>43353</v>
-      </c>
-      <c r="K2" s="54">
-        <v>43354</v>
-      </c>
-      <c r="L2" s="54">
-        <v>43356</v>
-      </c>
-      <c r="M2" s="54">
-        <v>43357</v>
+      <c r="J2" s="54" t="s">
+        <v>26</v>
+      </c>
+      <c r="K2" s="54" t="s">
+        <v>27</v>
+      </c>
+      <c r="L2" s="54" t="s">
+        <v>28</v>
+      </c>
+      <c r="M2" s="54" t="s">
+        <v>29</v>
       </c>
       <c r="N2" s="54"/>
       <c r="O2" s="54">
@@ -1599,7 +1612,7 @@
       <c r="C3" s="40"/>
       <c r="D3" s="16"/>
       <c r="E3" s="73" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F3" s="73" t="s">
         <v>3</v>
@@ -1607,12 +1620,22 @@
       <c r="G3" s="73" t="s">
         <v>10</v>
       </c>
-      <c r="H3" s="73"/>
+      <c r="H3" s="73" t="s">
+        <v>10</v>
+      </c>
       <c r="I3" s="73"/>
-      <c r="J3" s="73"/>
-      <c r="K3" s="73"/>
-      <c r="L3" s="73"/>
-      <c r="M3" s="73"/>
+      <c r="J3" s="73" t="s">
+        <v>11</v>
+      </c>
+      <c r="K3" s="73" t="s">
+        <v>3</v>
+      </c>
+      <c r="L3" s="73" t="s">
+        <v>3</v>
+      </c>
+      <c r="M3" s="73" t="s">
+        <v>3</v>
+      </c>
       <c r="N3" s="73"/>
       <c r="O3" s="73"/>
       <c r="P3" s="73"/>
@@ -1708,12 +1731,22 @@
       <c r="G4" s="73" t="s">
         <v>11</v>
       </c>
-      <c r="H4" s="73"/>
+      <c r="H4" s="73" t="s">
+        <v>3</v>
+      </c>
       <c r="I4" s="73"/>
-      <c r="J4" s="73"/>
-      <c r="K4" s="73"/>
-      <c r="L4" s="73"/>
-      <c r="M4" s="73"/>
+      <c r="J4" s="73" t="s">
+        <v>3</v>
+      </c>
+      <c r="K4" s="73" t="s">
+        <v>11</v>
+      </c>
+      <c r="L4" s="73" t="s">
+        <v>11</v>
+      </c>
+      <c r="M4" s="73" t="s">
+        <v>11</v>
+      </c>
       <c r="N4" s="73"/>
       <c r="O4" s="73"/>
       <c r="P4" s="73"/>
@@ -1809,12 +1842,22 @@
       <c r="G5" s="73" t="s">
         <v>3</v>
       </c>
-      <c r="H5" s="73"/>
+      <c r="H5" s="73" t="s">
+        <v>3</v>
+      </c>
       <c r="I5" s="73"/>
-      <c r="J5" s="73"/>
-      <c r="K5" s="73"/>
-      <c r="L5" s="73"/>
-      <c r="M5" s="73"/>
+      <c r="J5" s="73" t="s">
+        <v>3</v>
+      </c>
+      <c r="K5" s="73" t="s">
+        <v>3</v>
+      </c>
+      <c r="L5" s="73" t="s">
+        <v>3</v>
+      </c>
+      <c r="M5" s="73" t="s">
+        <v>3</v>
+      </c>
       <c r="N5" s="73"/>
       <c r="O5" s="73"/>
       <c r="P5" s="73"/>
@@ -1910,12 +1953,22 @@
       <c r="G6" s="73" t="s">
         <v>3</v>
       </c>
-      <c r="H6" s="73"/>
+      <c r="H6" s="73" t="s">
+        <v>11</v>
+      </c>
       <c r="I6" s="73"/>
-      <c r="J6" s="73"/>
-      <c r="K6" s="73"/>
-      <c r="L6" s="73"/>
-      <c r="M6" s="73"/>
+      <c r="J6" s="73" t="s">
+        <v>10</v>
+      </c>
+      <c r="K6" s="73" t="s">
+        <v>3</v>
+      </c>
+      <c r="L6" s="73" t="s">
+        <v>11</v>
+      </c>
+      <c r="M6" s="73" t="s">
+        <v>3</v>
+      </c>
       <c r="N6" s="73"/>
       <c r="O6" s="73"/>
       <c r="P6" s="73"/>
@@ -2011,12 +2064,22 @@
       <c r="G7" s="74" t="s">
         <v>3</v>
       </c>
-      <c r="H7" s="74"/>
+      <c r="H7" s="74" t="s">
+        <v>11</v>
+      </c>
       <c r="I7" s="74"/>
-      <c r="J7" s="74"/>
-      <c r="K7" s="74"/>
-      <c r="L7" s="74"/>
-      <c r="M7" s="74"/>
+      <c r="J7" s="74" t="s">
+        <v>10</v>
+      </c>
+      <c r="K7" s="74" t="s">
+        <v>11</v>
+      </c>
+      <c r="L7" s="74" t="s">
+        <v>3</v>
+      </c>
+      <c r="M7" s="74" t="s">
+        <v>11</v>
+      </c>
       <c r="N7" s="74"/>
       <c r="O7" s="74"/>
       <c r="P7" s="74"/>
@@ -2436,23 +2499,23 @@
       </c>
       <c r="E18" s="19">
         <f>COUNTIF(E3:AV3,"v")</f>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F18" s="20">
         <f>COUNTIF(E4:AV4,"v")</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G18" s="20">
         <f>COUNTIF(E5:AV5,"v")</f>
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="H18" s="20">
         <f>COUNTIF(E6:AV6,"v")</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="I18" s="21">
         <f>COUNTIF(F7:AW7,"v")</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R18"/>
     </row>
@@ -2494,7 +2557,7 @@
       </c>
       <c r="E20" s="25">
         <f>COUNTIF(E3:AQ3,"c")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F20" s="26">
         <f>COUNTIF(E4:AQ4,"c")</f>
@@ -2552,11 +2615,11 @@
       </c>
       <c r="E22" s="28">
         <f>COUNTIF(E3:AQ3,"t")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F22" s="29">
         <f>COUNTIF(E4:AQ4,"t")</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G22" s="29">
         <f>COUNTIF(E5:AQ5,"t")</f>
@@ -2564,11 +2627,11 @@
       </c>
       <c r="H22" s="29">
         <f>COUNTIF(E6:AV6,"t")</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I22" s="30">
         <f>COUNTIF(F7:AW7,"t")</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="R22" s="5"/>
     </row>
@@ -2581,7 +2644,7 @@
       </c>
       <c r="E23" s="31">
         <f>COUNTIF(E3:AQ3,"z")</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F23" s="32">
         <f>COUNTIF(E4:AQ4,"z")</f>
@@ -2593,11 +2656,11 @@
       </c>
       <c r="H23" s="32">
         <f>COUNTIF(E6:AQ6,"z")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I23" s="33">
         <f>COUNTIF(E7:AR7,"z")</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="R23" s="5"/>
     </row>

</xml_diff>